<commit_message>
files added from running the full notebook
</commit_message>
<xml_diff>
--- a/Summary of All done so Far/final_steel_data.xlsx
+++ b/Summary of All done so Far/final_steel_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -552,7 +552,7 @@
         <v>-1.490660174789605</v>
       </c>
       <c r="G2" t="n">
-        <v>1.827393979612947</v>
+        <v>1.827393979612949</v>
       </c>
       <c r="H2" t="n">
         <v>0.1009407378333902</v>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-2.189442802529632</v>
+        <v>-2.18944280252963</v>
       </c>
       <c r="C3" t="n">
         <v>0.7646474317006144</v>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1.925643029316244</v>
+        <v>-1.925643029316248</v>
       </c>
       <c r="C6" t="n">
         <v>-0.7968400041437843</v>
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-1.686271782138614</v>
+        <v>-1.686271782138617</v>
       </c>
       <c r="C7" t="n">
         <v>0.8564996338091085</v>
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-1.854010506857741</v>
+        <v>-1.854010506857738</v>
       </c>
       <c r="C8" t="n">
         <v>-0.8886922062522783</v>
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1.867777052688738</v>
+        <v>-1.867777052688737</v>
       </c>
       <c r="C9" t="n">
         <v>0.02982981483266219</v>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1.156123118905282</v>
+        <v>-1.156123118905287</v>
       </c>
       <c r="C10" t="n">
         <v>-0.7968400041437843</v>
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1.591997874049647</v>
+        <v>-1.591997874049649</v>
       </c>
       <c r="C11" t="n">
         <v>0.5809430274836264</v>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1.754485053560486</v>
+        <v>-1.754485053560484</v>
       </c>
       <c r="C12" t="n">
         <v>-0.7968400041437843</v>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-1.462116315011992</v>
+        <v>-1.462116315011989</v>
       </c>
       <c r="C14" t="n">
         <v>0.5809430274836264</v>
@@ -1354,7 +1354,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.663010351745686</v>
+        <v>-1.663010351745683</v>
       </c>
       <c r="C15" t="n">
         <v>-0.8886922062522783</v>
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.558621529890734</v>
+        <v>-1.558621529890731</v>
       </c>
       <c r="C16" t="n">
         <v>0.5809430274836264</v>
@@ -1606,7 +1606,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-1.312907487131709</v>
+        <v>-1.312907487131706</v>
       </c>
       <c r="C19" t="n">
         <v>0.5809430274836264</v>
@@ -1669,7 +1669,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-1.723600604162418</v>
+        <v>-1.723600604162415</v>
       </c>
       <c r="C20" t="n">
         <v>-0.7968400041437843</v>
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.929009490350575</v>
+        <v>-0.9290094903505777</v>
       </c>
       <c r="C21" t="n">
         <v>-0.7968400041437843</v>
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1.500612435316005</v>
+        <v>-1.500612435316007</v>
       </c>
       <c r="C22" t="n">
         <v>-0.7968400041437843</v>
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-1.536664311721083</v>
+        <v>-1.536664311721081</v>
       </c>
       <c r="C23" t="n">
         <v>-0.7968400041437843</v>
@@ -1921,7 +1921,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-1.350494885695844</v>
+        <v>-1.350494885695847</v>
       </c>
       <c r="C24" t="n">
         <v>-0.2457267914928199</v>
@@ -1984,7 +1984,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-1.290310758985587</v>
+        <v>-1.290310758985585</v>
       </c>
       <c r="C25" t="n">
         <v>0.5809430274836264</v>
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-1.337053264020127</v>
+        <v>-1.33705326402013</v>
       </c>
       <c r="C26" t="n">
         <v>0.5809430274836264</v>
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-1.258473501674028</v>
+        <v>-1.258473501674025</v>
       </c>
       <c r="C28" t="n">
         <v>-0.7968400041437843</v>
@@ -2188,7 +2188,7 @@
         <v>0.5679643270913278</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.02344304616547688</v>
+        <v>-0.0234430461654766</v>
       </c>
       <c r="H28" t="n">
         <v>1.213984647858924</v>
@@ -2614,7 +2614,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-1.201929909547983</v>
+        <v>-1.201929909547986</v>
       </c>
       <c r="C35" t="n">
         <v>-0.7968400041437843</v>
@@ -2656,7 +2656,7 @@
         <v>-0.5376450060571849</v>
       </c>
       <c r="P35" t="n">
-        <v>1832.446958858221</v>
+        <v>1832.446958858228</v>
       </c>
       <c r="Q35" t="n">
         <v>1953.3</v>
@@ -2677,7 +2677,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-1.033960319801774</v>
+        <v>-1.033960319801771</v>
       </c>
       <c r="C36" t="n">
         <v>1.040204038026096</v>
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-1.196055241162636</v>
+        <v>-1.196055241162633</v>
       </c>
       <c r="C37" t="n">
         <v>-0.8886922062522783</v>
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-0.811675866649793</v>
+        <v>-0.8116758666497956</v>
       </c>
       <c r="C40" t="n">
         <v>1.040204038026096</v>
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-1.65621620697855</v>
+        <v>-1.656216206978548</v>
       </c>
       <c r="C41" t="n">
         <v>-0.06202238727583193</v>
@@ -3370,7 +3370,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.9684045374650506</v>
+        <v>-0.9684045374650453</v>
       </c>
       <c r="C47" t="n">
         <v>0.9483518359176026</v>
@@ -3433,7 +3433,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-1.237157511217596</v>
+        <v>-1.237157511217593</v>
       </c>
       <c r="C48" t="n">
         <v>0.02982981483266219</v>
@@ -3559,7 +3559,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-1.279667411949067</v>
+        <v>-1.279667411949069</v>
       </c>
       <c r="C50" t="n">
         <v>-0.7968400041437843</v>
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-1.277685539151353</v>
+        <v>-1.277685539151351</v>
       </c>
       <c r="C51" t="n">
         <v>-0.7968400041437843</v>
@@ -3811,7 +3811,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-0.922757857655801</v>
+        <v>-0.9227578576557983</v>
       </c>
       <c r="C54" t="n">
         <v>0.9483518359176026</v>
@@ -3874,7 +3874,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.9958332935219053</v>
+        <v>-0.995833293521908</v>
       </c>
       <c r="C55" t="n">
         <v>1.315760644351579</v>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-1.094480996161682</v>
+        <v>-1.094480996161684</v>
       </c>
       <c r="C56" t="n">
         <v>0.4890908253751323</v>
@@ -4063,7 +4063,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-1.276204655709009</v>
+        <v>-1.276204655709004</v>
       </c>
       <c r="C58" t="n">
         <v>-0.7968400041437843</v>
@@ -4189,7 +4189,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.8991806446051824</v>
+        <v>-0.8991806446051851</v>
       </c>
       <c r="C60" t="n">
         <v>-0.7968400041437843</v>
@@ -4250,7 +4250,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.9941462014153448</v>
+        <v>-0.9941462014153422</v>
       </c>
       <c r="C61" t="n">
         <v>-0.06202238727583193</v>
@@ -4376,7 +4376,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-0.8771027935309216</v>
+        <v>-0.8771027935309244</v>
       </c>
       <c r="C63" t="n">
         <v>-0.8886922062522783</v>
@@ -4581,7 +4581,7 @@
         <v>-1.28995588200899</v>
       </c>
       <c r="H66" t="n">
-        <v>0.1320829862127196</v>
+        <v>0.1320829862127201</v>
       </c>
       <c r="I66" t="n">
         <v>1.736893329911471</v>
@@ -4689,7 +4689,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-0.9191875255566807</v>
+        <v>-0.919187525556678</v>
       </c>
       <c r="C68" t="n">
         <v>0.1216820169411562</v>
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.7376384488295903</v>
+        <v>-0.737638448829593</v>
       </c>
       <c r="C69" t="n">
         <v>0.8564996338091085</v>
@@ -4815,7 +4815,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.7688372977138078</v>
+        <v>-0.7688372977138052</v>
       </c>
       <c r="C70" t="n">
         <v>0.9483518359176026</v>
@@ -4842,7 +4842,7 @@
         <v>-0.3034984966852858</v>
       </c>
       <c r="K70" t="n">
-        <v>0.2757276658928732</v>
+        <v>0.2757276658928733</v>
       </c>
       <c r="L70" t="n">
         <v>1.302430692972525</v>
@@ -5193,7 +5193,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.6477168583743147</v>
+        <v>-0.6477168583743174</v>
       </c>
       <c r="C76" t="n">
         <v>0.9483518359176026</v>
@@ -5319,7 +5319,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.619257047395666</v>
+        <v>-0.6192570473956687</v>
       </c>
       <c r="C78" t="n">
         <v>1.132056240134591</v>
@@ -5508,7 +5508,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-0.7781286632209305</v>
+        <v>-0.7781286632209332</v>
       </c>
       <c r="C81" t="n">
         <v>-0.7968400041437843</v>
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-1.115548809541203</v>
+        <v>-1.115548809541201</v>
       </c>
       <c r="C83" t="n">
         <v>-0.7968400041437843</v>
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-1.144597263010343</v>
+        <v>-1.14459726301034</v>
       </c>
       <c r="C91" t="n">
         <v>-0.5212833978183021</v>
@@ -6636,7 +6636,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-0.6781383063339746</v>
+        <v>-0.6781383063339719</v>
       </c>
       <c r="C99" t="n">
         <v>1.132056240134591</v>
@@ -6762,7 +6762,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-0.5020014441531647</v>
+        <v>-0.5020014441531594</v>
       </c>
       <c r="C101" t="n">
         <v>1.223908442243085</v>
@@ -6888,7 +6888,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-0.4928932719791498</v>
+        <v>-0.4928932719791471</v>
       </c>
       <c r="C103" t="n">
         <v>0.8564996338091085</v>
@@ -7014,7 +7014,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-0.5172054111174322</v>
+        <v>-0.5172054111174349</v>
       </c>
       <c r="C105" t="n">
         <v>1.040204038026096</v>
@@ -7077,7 +7077,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-0.4967311937482877</v>
+        <v>-0.496731193748285</v>
       </c>
       <c r="C106" t="n">
         <v>1.040204038026096</v>
@@ -7140,7 +7140,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-0.8574349761992118</v>
+        <v>-0.8574349761992092</v>
       </c>
       <c r="C107" t="n">
         <v>-0.7968400041437843</v>
@@ -7266,7 +7266,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-0.8689179087309078</v>
+        <v>-0.868917908730905</v>
       </c>
       <c r="C109" t="n">
         <v>-0.7968400041437843</v>
@@ -7329,7 +7329,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-0.4408741796816212</v>
+        <v>-0.440874179681624</v>
       </c>
       <c r="C110" t="n">
         <v>0.9483518359176026</v>
@@ -7455,7 +7455,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.6360275941574595</v>
+        <v>-0.6360275941574621</v>
       </c>
       <c r="C112" t="n">
         <v>-0.7049878020352901</v>
@@ -7707,7 +7707,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-0.1100502207876473</v>
+        <v>-0.11005022078765</v>
       </c>
       <c r="C116" t="n">
         <v>-0.7049878020352901</v>
@@ -7770,7 +7770,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-0.195997619685546</v>
+        <v>-0.1959976196855434</v>
       </c>
       <c r="C117" t="n">
         <v>-0.337578993601314</v>
@@ -7782,7 +7782,7 @@
         <v>0.1689764000890147</v>
       </c>
       <c r="F117" t="n">
-        <v>1.539674960803067</v>
+        <v>1.539674960803069</v>
       </c>
       <c r="G117" t="n">
         <v>-0.4772017538075347</v>
@@ -7833,7 +7833,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.4298796070749576</v>
+        <v>-0.4298796070749549</v>
       </c>
       <c r="C118" t="n">
         <v>0.8564996338091085</v>
@@ -7959,7 +7959,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.7125104206648332</v>
+        <v>-0.7125104206648359</v>
       </c>
       <c r="C120" t="n">
         <v>-0.7968400041437843</v>
@@ -8022,7 +8022,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.69444522622379</v>
+        <v>-0.6944452262237927</v>
       </c>
       <c r="C121" t="n">
         <v>-0.7968400041437843</v>
@@ -8085,7 +8085,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.01421857701933621</v>
+        <v>-0.01421857701933891</v>
       </c>
       <c r="C122" t="n">
         <v>-0.7049878020352901</v>
@@ -8274,7 +8274,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.7610895539255397</v>
+        <v>-0.761089553925537</v>
       </c>
       <c r="C125" t="n">
         <v>-0.7049878020352901</v>
@@ -8337,7 +8337,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.768524696138447</v>
+        <v>-0.7685246961384442</v>
       </c>
       <c r="C126" t="n">
         <v>-0.7049878020352901</v>
@@ -8463,7 +8463,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.4156916063557646</v>
+        <v>-0.4156916063557672</v>
       </c>
       <c r="C128" t="n">
         <v>1.132056240134591</v>
@@ -8589,7 +8589,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.3011747977549318</v>
+        <v>-0.3011747977549344</v>
       </c>
       <c r="C130" t="n">
         <v>0.4890908253751323</v>
@@ -8715,7 +8715,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-0.3722931614693307</v>
+        <v>-0.3722931614693334</v>
       </c>
       <c r="C132" t="n">
         <v>1.223908442243085</v>
@@ -8778,7 +8778,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.550005836621087</v>
+        <v>-0.5500058366210844</v>
       </c>
       <c r="C133" t="n">
         <v>-0.6131355999267961</v>
@@ -8904,7 +8904,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-0.4428319936904363</v>
+        <v>-0.442831993690439</v>
       </c>
       <c r="C135" t="n">
         <v>0.02982981483266219</v>
@@ -8967,7 +8967,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-0.3655659156817216</v>
+        <v>-0.3655659156817244</v>
       </c>
       <c r="C136" t="n">
         <v>1.132056240134591</v>
@@ -9030,7 +9030,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>-0.3435398557978432</v>
+        <v>-0.3435398557978459</v>
       </c>
       <c r="C137" t="n">
         <v>1.040204038026096</v>
@@ -9093,7 +9093,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.3320359470996054</v>
+        <v>-0.332035947099608</v>
       </c>
       <c r="C138" t="n">
         <v>1.223908442243085</v>
@@ -9282,7 +9282,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-0.05010006538969593</v>
+        <v>-0.05010006538969863</v>
       </c>
       <c r="C141" t="n">
         <v>-0.6131355999267961</v>
@@ -9345,7 +9345,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.3252774690901798</v>
+        <v>-0.3252774690901825</v>
       </c>
       <c r="C142" t="n">
         <v>1.040204038026096</v>
@@ -9471,7 +9471,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.4084132337446963</v>
+        <v>-0.408413233744699</v>
       </c>
       <c r="C144" t="n">
         <v>-0.1538745893843259</v>
@@ -9597,7 +9597,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>-0.3643180266580241</v>
+        <v>-0.3643180266580214</v>
       </c>
       <c r="C146" t="n">
         <v>-0.7968400041437843</v>
@@ -9723,7 +9723,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-0.3515621862798432</v>
+        <v>-0.3515621862798459</v>
       </c>
       <c r="C148" t="n">
         <v>-0.7049878020352901</v>
@@ -9786,7 +9786,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>-0.3800863195634054</v>
+        <v>-0.3800863195634081</v>
       </c>
       <c r="C149" t="n">
         <v>-0.7049878020352901</v>
@@ -9849,7 +9849,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.2532577857643359</v>
+        <v>0.2532577857643386</v>
       </c>
       <c r="C150" t="n">
         <v>-0.06202238727583193</v>
@@ -9912,7 +9912,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-0.402545153914996</v>
+        <v>-0.4025451539149906</v>
       </c>
       <c r="C151" t="n">
         <v>-0.7968400041437843</v>
@@ -10101,7 +10101,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-0.3090829351641279</v>
+        <v>-0.3090829351641252</v>
       </c>
       <c r="C154" t="n">
         <v>-0.5212833978183021</v>
@@ -10290,7 +10290,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.3665537122722808</v>
+        <v>-0.3665537122722754</v>
       </c>
       <c r="C157" t="n">
         <v>-0.7968400041437843</v>
@@ -10479,7 +10479,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>-0.08495860838946298</v>
+        <v>-0.08495860838946567</v>
       </c>
       <c r="C160" t="n">
         <v>-0.6131355999267961</v>
@@ -10605,7 +10605,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-0.2883738600371383</v>
+        <v>-0.2883738600371357</v>
       </c>
       <c r="C162" t="n">
         <v>-0.7968400041437843</v>
@@ -10668,7 +10668,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.2304405078301133</v>
+        <v>0.230440507830116</v>
       </c>
       <c r="C163" t="n">
         <v>-0.06202238727583193</v>
@@ -10794,7 +10794,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.2255218811147812</v>
+        <v>0.2255218811147785</v>
       </c>
       <c r="C165" t="n">
         <v>-0.06202238727583193</v>
@@ -10920,7 +10920,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.01736540024888934</v>
+        <v>0.01736540024888665</v>
       </c>
       <c r="C167" t="n">
         <v>0.5809430274836264</v>
@@ -10983,7 +10983,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.04168016365492313</v>
+        <v>0.04168016365492044</v>
       </c>
       <c r="C168" t="n">
         <v>0.5809430274836264</v>
@@ -11172,7 +11172,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.2154347458153269</v>
+        <v>0.2154347458153242</v>
       </c>
       <c r="C171" t="n">
         <v>1.315760644351579</v>
@@ -11235,7 +11235,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.2293648589845682</v>
+        <v>0.2293648589845655</v>
       </c>
       <c r="C172" t="n">
         <v>1.223908442243085</v>
@@ -11298,7 +11298,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>-0.1706415360077047</v>
+        <v>-0.170641536007702</v>
       </c>
       <c r="C173" t="n">
         <v>-0.7049878020352901</v>
@@ -11424,7 +11424,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.2507471005540547</v>
+        <v>0.2507471005540521</v>
       </c>
       <c r="C175" t="n">
         <v>1.315760644351579</v>
@@ -11487,7 +11487,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.5230982360133076</v>
+        <v>0.523098236013305</v>
       </c>
       <c r="C176" t="n">
         <v>0.02982981483266219</v>
@@ -11499,7 +11499,7 @@
         <v>0.1345307193150829</v>
       </c>
       <c r="F176" t="n">
-        <v>1.645994559986937</v>
+        <v>1.645994559986935</v>
       </c>
       <c r="G176" t="n">
         <v>-0.6261274615091659</v>
@@ -11550,7 +11550,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.1823933753624469</v>
+        <v>0.1823933753624496</v>
       </c>
       <c r="C177" t="n">
         <v>0.4890908253751323</v>
@@ -11928,7 +11928,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.5864838324922033</v>
+        <v>0.5864838324922059</v>
       </c>
       <c r="C183" t="n">
         <v>-0.5212833978183021</v>
@@ -12054,7 +12054,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.6045693149332095</v>
+        <v>0.6045693149332068</v>
       </c>
       <c r="C185" t="n">
         <v>-0.6131355999267961</v>
@@ -12117,7 +12117,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.6049751266203821</v>
+        <v>0.6049751266203794</v>
       </c>
       <c r="C186" t="n">
         <v>-0.6131355999267961</v>
@@ -12243,7 +12243,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.5899786093960594</v>
+        <v>0.5899786093960566</v>
       </c>
       <c r="C188" t="n">
         <v>-0.6131355999267961</v>
@@ -12495,7 +12495,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.3452321293762594</v>
+        <v>0.3452321293762567</v>
       </c>
       <c r="C192" t="n">
         <v>0.2135342190496502</v>
@@ -12558,7 +12558,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.6183223588929694</v>
+        <v>0.6183223588929667</v>
       </c>
       <c r="C193" t="n">
         <v>-0.6131355999267961</v>
@@ -12621,7 +12621,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.6149059700895604</v>
+        <v>0.6149059700895577</v>
       </c>
       <c r="C194" t="n">
         <v>-0.6131355999267961</v>
@@ -12873,7 +12873,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.6269126419395052</v>
+        <v>0.6269126419395026</v>
       </c>
       <c r="C198" t="n">
         <v>-0.6131355999267961</v>
@@ -12999,7 +12999,7 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.6443429736254097</v>
+        <v>0.6443429736254124</v>
       </c>
       <c r="C200" t="n">
         <v>-0.5212833978183021</v>
@@ -13062,7 +13062,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.6515663700955018</v>
+        <v>0.6515663700955044</v>
       </c>
       <c r="C201" t="n">
         <v>0.3053864211581443</v>
@@ -13125,7 +13125,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.7774514341912458</v>
+        <v>0.7774514341912486</v>
       </c>
       <c r="C202" t="n">
         <v>0.3972386232666384</v>
@@ -13251,7 +13251,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.6984710144086335</v>
+        <v>0.6984710144086307</v>
       </c>
       <c r="C204" t="n">
         <v>0.2135342190496502</v>
@@ -13314,7 +13314,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.5893695334238446</v>
+        <v>0.5893695334238473</v>
       </c>
       <c r="C205" t="n">
         <v>-0.7968400041437843</v>
@@ -13566,7 +13566,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.6973050994395451</v>
+        <v>0.6973050994395423</v>
       </c>
       <c r="C209" t="n">
         <v>-0.5212833978183021</v>
@@ -13755,7 +13755,7 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.572466429215418</v>
+        <v>0.5724664292154233</v>
       </c>
       <c r="C212" t="n">
         <v>-0.7968400041437843</v>
@@ -13944,7 +13944,7 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>0.2723719625386873</v>
+        <v>0.27237196253869</v>
       </c>
       <c r="C215" t="n">
         <v>0.02982981483266219</v>
@@ -14007,7 +14007,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.727293221671123</v>
+        <v>0.7272932216711177</v>
       </c>
       <c r="C216" t="n">
         <v>-0.8886922062522783</v>
@@ -14259,7 +14259,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.7351699716262301</v>
+        <v>0.7351699716262328</v>
       </c>
       <c r="C220" t="n">
         <v>-0.8886922062522783</v>
@@ -14574,7 +14574,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.741256825455802</v>
+        <v>0.7412568254558046</v>
       </c>
       <c r="C225" t="n">
         <v>-0.8886922062522783</v>
@@ -14826,7 +14826,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.6958639620616514</v>
+        <v>0.6958639620616568</v>
       </c>
       <c r="C229" t="n">
         <v>-0.7968400041437843</v>
@@ -15141,7 +15141,7 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.8034356329416926</v>
+        <v>0.8034356329416953</v>
       </c>
       <c r="C234" t="n">
         <v>-0.8886922062522783</v>
@@ -15393,7 +15393,7 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.7777038307928292</v>
+        <v>0.7777038307928346</v>
       </c>
       <c r="C238" t="n">
         <v>-0.6131355999267961</v>
@@ -15519,7 +15519,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.8269435663049866</v>
+        <v>0.8269435663049892</v>
       </c>
       <c r="C240" t="n">
         <v>-0.7968400041437843</v>
@@ -15834,7 +15834,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.7582879202631866</v>
+        <v>0.7582879202631839</v>
       </c>
       <c r="C245" t="n">
         <v>-0.7049878020352901</v>
@@ -15897,7 +15897,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>1.103754517540001</v>
+        <v>1.103754517539999</v>
       </c>
       <c r="C246" t="n">
         <v>-0.6131355999267961</v>
@@ -15960,7 +15960,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.841433877343716</v>
+        <v>0.8414338773437132</v>
       </c>
       <c r="C247" t="n">
         <v>-0.6131355999267961</v>
@@ -16023,7 +16023,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.8399693588579336</v>
+        <v>0.8399693588579282</v>
       </c>
       <c r="C248" t="n">
         <v>-0.6131355999267961</v>
@@ -16086,7 +16086,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>1.293951024191677</v>
+        <v>1.293951024191682</v>
       </c>
       <c r="C249" t="n">
         <v>-0.7968400041437843</v>
@@ -16338,7 +16338,7 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>0.8592898130525898</v>
+        <v>0.859289813052587</v>
       </c>
       <c r="C253" t="n">
         <v>-0.6131355999267961</v>
@@ -16653,7 +16653,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>1.091477541839367</v>
+        <v>1.091477541839364</v>
       </c>
       <c r="C258" t="n">
         <v>-0.7049878020352901</v>
@@ -16758,7 +16758,7 @@
         <v>-0.1941544368490276</v>
       </c>
       <c r="P259" t="n">
-        <v>1366.189766049129</v>
+        <v>1366.189766049128</v>
       </c>
       <c r="Q259" t="n">
         <v>1429</v>
@@ -16905,7 +16905,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.9521968454010715</v>
+        <v>0.9521968454010687</v>
       </c>
       <c r="C262" t="n">
         <v>1.775021654894049</v>
@@ -16968,7 +16968,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>0.810681685404276</v>
+        <v>0.8106816854042787</v>
       </c>
       <c r="C263" t="n">
         <v>-0.6131355999267961</v>
@@ -17094,7 +17094,7 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>1.113454449835316</v>
+        <v>1.113454449835314</v>
       </c>
       <c r="C265" t="n">
         <v>-0.7968400041437843</v>
@@ -17157,7 +17157,7 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>1.180262160234859</v>
+        <v>1.180262160234861</v>
       </c>
       <c r="C266" t="n">
         <v>-0.7968400041437843</v>
@@ -17283,7 +17283,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>1.189575136103749</v>
+        <v>1.189575136103752</v>
       </c>
       <c r="C268" t="n">
         <v>-0.6131355999267961</v>
@@ -17472,7 +17472,7 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>1.249213932290817</v>
+        <v>1.249213932290814</v>
       </c>
       <c r="C271" t="n">
         <v>-0.7968400041437843</v>
@@ -17535,7 +17535,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>1.269739483666128</v>
+        <v>1.26973948366613</v>
       </c>
       <c r="C272" t="n">
         <v>-0.7968400041437843</v>
@@ -17661,7 +17661,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>1.24048576794642</v>
+        <v>1.240485767946417</v>
       </c>
       <c r="C274" t="n">
         <v>-0.7968400041437843</v>
@@ -17724,7 +17724,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>1.199701479237695</v>
+        <v>1.19970147923769</v>
       </c>
       <c r="C275" t="n">
         <v>-0.7968400041437843</v>
@@ -17787,7 +17787,7 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>1.29504132988526</v>
+        <v>1.295041329885263</v>
       </c>
       <c r="C276" t="n">
         <v>-0.7049878020352901</v>
@@ -17913,7 +17913,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>1.283500272467852</v>
+        <v>1.28350027246785</v>
       </c>
       <c r="C278" t="n">
         <v>-0.7968400041437843</v>
@@ -18039,7 +18039,7 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>1.347127920034419</v>
+        <v>1.347127920034422</v>
       </c>
       <c r="C280" t="n">
         <v>-0.7049878020352901</v>
@@ -18165,7 +18165,7 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>1.339520655438369</v>
+        <v>1.339520655438375</v>
       </c>
       <c r="C282" t="n">
         <v>-0.7968400041437843</v>
@@ -18354,7 +18354,7 @@
         </is>
       </c>
       <c r="B285" t="n">
-        <v>1.297906613643247</v>
+        <v>1.297906613643244</v>
       </c>
       <c r="C285" t="n">
         <v>-0.8886922062522783</v>
@@ -18417,7 +18417,7 @@
         </is>
       </c>
       <c r="B286" t="n">
-        <v>1.634153603485994</v>
+        <v>1.634153603485996</v>
       </c>
       <c r="C286" t="n">
         <v>-0.7968400041437843</v>
@@ -18480,7 +18480,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>1.29257993494534</v>
+        <v>1.292579934945338</v>
       </c>
       <c r="C287" t="n">
         <v>-0.7968400041437843</v>
@@ -18606,7 +18606,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>1.32738153964223</v>
+        <v>1.327381539642233</v>
       </c>
       <c r="C289" t="n">
         <v>2.509839271762001</v>
@@ -18777,10 +18777,10 @@
         <v>1688.1</v>
       </c>
       <c r="Q291" t="n">
-        <v>2076.345765086513</v>
+        <v>2076.345765086512</v>
       </c>
       <c r="R291" t="n">
-        <v>6.607534013147519</v>
+        <v>6.60753401314752</v>
       </c>
       <c r="S291" t="inlineStr">
         <is>
@@ -18858,7 +18858,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>1.39565159767469</v>
+        <v>1.395651597674693</v>
       </c>
       <c r="C293" t="n">
         <v>-0.7968400041437843</v>
@@ -19173,7 +19173,7 @@
         </is>
       </c>
       <c r="B298" t="n">
-        <v>1.521995777962169</v>
+        <v>1.521995777962166</v>
       </c>
       <c r="C298" t="n">
         <v>2.693543675978989</v>
@@ -19362,7 +19362,7 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>1.557687979109155</v>
+        <v>1.557687979109157</v>
       </c>
       <c r="C301" t="n">
         <v>-0.7049878020352901</v>
@@ -19425,7 +19425,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>1.534588105685619</v>
+        <v>1.534588105685622</v>
       </c>
       <c r="C302" t="n">
         <v>2.417987069653507</v>
@@ -19488,7 +19488,7 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>1.589966958149887</v>
+        <v>1.58996695814989</v>
       </c>
       <c r="C303" t="n">
         <v>-0.7049878020352901</v>
@@ -19614,7 +19614,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>1.880413387621373</v>
+        <v>1.880413387621376</v>
       </c>
       <c r="C305" t="n">
         <v>0.1216820169411562</v>
@@ -20055,7 +20055,7 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>2.591037648619276</v>
+        <v>2.591037648619273</v>
       </c>
       <c r="C312" t="n">
         <v>1.591317250677061</v>

</xml_diff>